<commit_message>
path_part working with hash table
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\deduper\super-duper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1528799D-976A-4094-89DD-C543BB4D28A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4B7C6C-FEED-42CE-86FF-25013810F1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B4F81478-EDC6-4AF2-8C94-8DECCD28A9F1}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
   <si>
     <t>id</t>
   </si>
@@ -236,6 +236,42 @@
   </si>
   <si>
     <t>Records / sec</t>
+  </si>
+  <si>
+    <t>Insert path_part</t>
+  </si>
+  <si>
+    <t>Input rows</t>
+  </si>
+  <si>
+    <t>Inserted rows</t>
+  </si>
+  <si>
+    <t>Crash</t>
+  </si>
+  <si>
+    <t>Chunk Size (Max = 65535 / Col Count (6))</t>
+  </si>
+  <si>
+    <t>Hashmap (no cap)</t>
+  </si>
+  <si>
+    <t>AHashmap (no cap)</t>
+  </si>
+  <si>
+    <t>Insert Time (ms)</t>
+  </si>
+  <si>
+    <t>Process Time</t>
+  </si>
+  <si>
+    <t>Process Rec/Sec</t>
+  </si>
+  <si>
+    <t>AHashmap (1255000)</t>
+  </si>
+  <si>
+    <t>Hashmap (1283850)</t>
   </si>
 </sst>
 </file>
@@ -244,8 +280,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -294,10 +330,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -633,31 +669,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8575576-B7CD-4022-B0CC-3DF2F1C8BE23}">
-  <dimension ref="B4:G12"/>
+  <dimension ref="B4:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>63</v>
       </c>
@@ -665,10 +705,10 @@
         <v>1025570</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>64</v>
       </c>
@@ -685,7 +725,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>59</v>
       </c>
@@ -693,11 +733,11 @@
         <v>499.65</v>
       </c>
       <c r="D9" s="3">
-        <f>C9/60</f>
+        <f t="shared" ref="D9:E12" si="0">C9/60</f>
         <v>8.3274999999999988</v>
       </c>
       <c r="E9" s="3">
-        <f>D9/60</f>
+        <f t="shared" si="0"/>
         <v>0.13879166666666665</v>
       </c>
       <c r="G9" s="4">
@@ -705,7 +745,7 @@
         <v>2052.576803762634</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>60</v>
       </c>
@@ -713,19 +753,19 @@
         <v>86488.75</v>
       </c>
       <c r="D10" s="3">
-        <f>C10/60</f>
+        <f t="shared" si="0"/>
         <v>1441.4791666666667</v>
       </c>
       <c r="E10" s="3">
-        <f>D10/60</f>
+        <f t="shared" si="0"/>
         <v>24.024652777777778</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" ref="G10:G12" si="0">$C$6/C10</f>
+        <f t="shared" ref="G10:G12" si="1">$C$6/C10</f>
         <v>11.857842783020914</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>61</v>
       </c>
@@ -733,19 +773,19 @@
         <v>1514.92</v>
       </c>
       <c r="D11" s="3">
-        <f>C11/60</f>
+        <f t="shared" si="0"/>
         <v>25.248666666666669</v>
       </c>
       <c r="E11" s="3">
-        <f>D11/60</f>
+        <f t="shared" si="0"/>
         <v>0.42081111111111114</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>676.9796424893724</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>62</v>
       </c>
@@ -753,16 +793,294 @@
         <v>283.02</v>
       </c>
       <c r="D12" s="3">
-        <f>C12/60</f>
+        <f t="shared" si="0"/>
         <v>4.7169999999999996</v>
       </c>
       <c r="E12" s="3">
-        <f>D12/60</f>
+        <f t="shared" si="0"/>
         <v>7.8616666666666654E-2</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3623.6661720019788</v>
+      </c>
+      <c r="Q12">
+        <f>P21/P20</f>
+        <v>1.2518063125871466</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <f>Q12*P20</f>
+        <v>1283815</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <f>65535/6</f>
+        <v>10922.5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="P19" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>72</v>
+      </c>
+      <c r="R19" t="s">
+        <v>77</v>
+      </c>
+      <c r="S19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20">
+        <v>30000</v>
+      </c>
+      <c r="D20">
+        <v>30000</v>
+      </c>
+      <c r="E20">
+        <v>30000</v>
+      </c>
+      <c r="F20">
+        <v>30000</v>
+      </c>
+      <c r="G20">
+        <v>30000</v>
+      </c>
+      <c r="H20">
+        <v>30000</v>
+      </c>
+      <c r="I20">
+        <v>30000</v>
+      </c>
+      <c r="J20">
+        <v>100000</v>
+      </c>
+      <c r="K20">
+        <v>100000</v>
+      </c>
+      <c r="L20">
+        <v>100000</v>
+      </c>
+      <c r="M20">
+        <v>250000</v>
+      </c>
+      <c r="N20">
+        <v>250000</v>
+      </c>
+      <c r="O20">
+        <v>250000</v>
+      </c>
+      <c r="P20">
+        <v>1025570</v>
+      </c>
+      <c r="Q20">
+        <v>1025570</v>
+      </c>
+      <c r="R20">
+        <v>1025570</v>
+      </c>
+      <c r="S20">
+        <v>1025570</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21">
+        <v>61825</v>
+      </c>
+      <c r="D21">
+        <v>61825</v>
+      </c>
+      <c r="F21">
+        <v>63270</v>
+      </c>
+      <c r="J21">
+        <v>174300</v>
+      </c>
+      <c r="K21">
+        <v>175232</v>
+      </c>
+      <c r="M21">
+        <v>382998</v>
+      </c>
+      <c r="N21">
+        <v>382877</v>
+      </c>
+      <c r="O21">
+        <v>382792</v>
+      </c>
+      <c r="P21">
+        <v>1283815</v>
+      </c>
+      <c r="Q21">
+        <v>1283815</v>
+      </c>
+      <c r="R21">
+        <v>1283815</v>
+      </c>
+      <c r="S21">
+        <v>1283815</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22">
+        <v>500</v>
+      </c>
+      <c r="D22">
+        <v>100</v>
+      </c>
+      <c r="E22">
+        <v>12000</v>
+      </c>
+      <c r="F22">
+        <v>10922</v>
+      </c>
+      <c r="G22">
+        <v>8000</v>
+      </c>
+      <c r="H22">
+        <v>7000</v>
+      </c>
+      <c r="I22">
+        <v>5000</v>
+      </c>
+      <c r="J22">
+        <v>10000</v>
+      </c>
+      <c r="K22">
+        <v>8000</v>
+      </c>
+      <c r="L22">
+        <v>5000</v>
+      </c>
+      <c r="M22">
+        <v>5000</v>
+      </c>
+      <c r="N22">
+        <v>10922</v>
+      </c>
+      <c r="O22">
+        <v>8000</v>
+      </c>
+      <c r="P22">
+        <v>10000</v>
+      </c>
+      <c r="Q22">
+        <v>10000</v>
+      </c>
+      <c r="R22">
+        <v>10000</v>
+      </c>
+      <c r="S22">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23">
+        <v>888</v>
+      </c>
+      <c r="D23">
+        <v>1065</v>
+      </c>
+      <c r="E23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23">
+        <v>784</v>
+      </c>
+      <c r="G23">
+        <v>779</v>
+      </c>
+      <c r="H23">
+        <v>795</v>
+      </c>
+      <c r="I23">
+        <v>793</v>
+      </c>
+      <c r="J23">
+        <v>2285</v>
+      </c>
+      <c r="K23">
+        <v>2215</v>
+      </c>
+      <c r="L23">
+        <v>2282</v>
+      </c>
+      <c r="M23">
+        <v>5124</v>
+      </c>
+      <c r="N23">
+        <v>5012</v>
+      </c>
+      <c r="O23">
+        <v>5073</v>
+      </c>
+      <c r="P23">
+        <v>17573</v>
+      </c>
+      <c r="Q23">
+        <v>17905</v>
+      </c>
+      <c r="R23">
+        <v>17616</v>
+      </c>
+      <c r="S23">
+        <v>17961</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="P24">
+        <v>16970</v>
+      </c>
+      <c r="Q24">
+        <v>15317</v>
+      </c>
+      <c r="R24">
+        <v>16067</v>
+      </c>
+      <c r="S24">
+        <v>15070</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="P25">
+        <v>80238.44</v>
+      </c>
+      <c r="Q25">
+        <v>85587</v>
+      </c>
+      <c r="R25">
+        <v>80238.44</v>
+      </c>
+      <c r="S25">
+        <v>85587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>